<commit_message>
Updated BrickChance excel sheet
</commit_message>
<xml_diff>
--- a/BrickChance.xlsx
+++ b/BrickChance.xlsx
@@ -8,17 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ae3ed2b53ee05886/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="8_{EA9B6267-12FA-4C99-AE1A-688634A55767}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F3EFFAC1-F1E8-4082-AE32-CF3EEE5BEC93}"/>
+  <xr:revisionPtr revIDLastSave="86" documentId="8_{EA9B6267-12FA-4C99-AE1A-688634A55767}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{03FBBA76-AC63-4044-9FF8-04CD1AF1CF91}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13695" xr2:uid="{C60DBB49-E795-4D1C-BA5F-40ABD00A5734}"/>
   </bookViews>
   <sheets>
-    <sheet name="BrickChanceGraph" sheetId="2" r:id="rId1"/>
+    <sheet name="BrickChanceGraph" sheetId="3" r:id="rId1"/>
     <sheet name="BrickChanceData" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="3" r:id="rId3"/>
+    <pivotCache cacheId="0" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -90,13 +90,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -157,7 +156,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t> that every rare candy is in the prize pool (brick chance)</a:t>
+              <a:t> of bricks when all rare candies are in the prize deck</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -309,16 +308,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.18</c:v>
+                  <c:v>10.31</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.03</c:v>
+                  <c:v>0.86999998999999995</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0.01</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.01</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -326,7 +325,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-DA12-4BBE-8FA0-6E0BD190DADB}"/>
+              <c16:uniqueId val="{00000000-7772-4032-AE39-34CCC71B07AE}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -339,11 +338,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="1536112"/>
-        <c:axId val="1540912"/>
+        <c:axId val="1077745647"/>
+        <c:axId val="1014335215"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1536112"/>
+        <c:axId val="1077745647"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -386,7 +385,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1540912"/>
+        <c:crossAx val="1014335215"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -394,7 +393,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1540912"/>
+        <c:axId val="1014335215"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -445,7 +444,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1536112"/>
+        <c:crossAx val="1077745647"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -527,7 +526,7 @@
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup orientation="landscape"/>
+    <c:pageSetup/>
   </c:printSettings>
   <c:extLst>
     <c:ext xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" uri="{781A3756-C4B2-4CAC-9D66-4F8BD8637D16}">
@@ -1109,22 +1108,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>597693</xdr:colOff>
+      <xdr:colOff>440530</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>135731</xdr:rowOff>
+      <xdr:rowOff>178593</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>635793</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>164306</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>259555</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>26193</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{186D0945-164E-0E85-54FB-0CDF8DB071AF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DEA8534D-EC35-905B-546A-E174104A1E4D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1145,8 +1144,12 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Rachel Hussmann" refreshedDate="45704.770843402781" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="4" xr:uid="{0DE04716-4335-439D-99DE-5B2DBFE875D1}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Rachel Hussmann" refreshedDate="45710.883911458332" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="4" xr:uid="{F46F0647-2605-4519-BF97-B3B47AA6F94F}">
   <cacheSource type="worksheet">
     <worksheetSource ref="A1:B5" sheet="BrickChanceData"/>
   </cacheSource>
@@ -1160,7 +1163,7 @@
       </sharedItems>
     </cacheField>
     <cacheField name="Percentage that every rare candy is in the prize pool" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="0.01" maxValue="0.18"/>
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="0" maxValue="10.31"/>
     </cacheField>
   </cacheFields>
   <extLst>
@@ -1175,11 +1178,11 @@
 <pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="4">
   <r>
     <x v="0"/>
-    <n v="0.18"/>
+    <n v="10.31"/>
   </r>
   <r>
     <x v="1"/>
-    <n v="0.03"/>
+    <n v="0.86999998999999995"/>
   </r>
   <r>
     <x v="2"/>
@@ -1187,13 +1190,13 @@
   </r>
   <r>
     <x v="3"/>
-    <n v="0.01"/>
+    <n v="0"/>
   </r>
 </pivotCacheRecords>
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{EDA2B7A6-D523-4688-8196-6FE4E67E9D85}" name="PivotTable1" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C6D48643-1AAB-4483-A901-59B1F906C505}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="2">
   <location ref="A3:B8" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="2">
     <pivotField axis="axisRow" showAll="0">
@@ -1572,17 +1575,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1F988A9-3664-4CBA-971E-FAA14D9B19CA}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56FEBFD4-B80C-4369-B39B-E0B3CEE7E724}">
   <dimension ref="A3:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N19" sqref="N19"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="11.9296875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="47.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="14.73046875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.86328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:2" x14ac:dyDescent="0.45">
@@ -1597,23 +1602,23 @@
       <c r="A4" s="2">
         <v>1</v>
       </c>
-      <c r="B4" s="3">
-        <v>0.18</v>
+      <c r="B4">
+        <v>10.31</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5" s="2">
         <v>2</v>
       </c>
-      <c r="B5" s="3">
-        <v>0.03</v>
+      <c r="B5">
+        <v>0.86999998999999995</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6" s="2">
         <v>3</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6">
         <v>0.01</v>
       </c>
     </row>
@@ -1621,22 +1626,21 @@
       <c r="A7" s="2">
         <v>4</v>
       </c>
-      <c r="B7" s="3">
-        <v>0.01</v>
+      <c r="B7">
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A8" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="3">
-        <v>0.23</v>
+      <c r="B8">
+        <v>11.18999999</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
-  <drawing r:id="rId3"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1667,7 +1671,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>0.18</v>
+        <v>10.31</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.45">
@@ -1675,7 +1679,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>0.03</v>
+        <v>0.86999998999999995</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.45">
@@ -1691,7 +1695,7 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>0.01</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>